<commit_message>
Add new disease files and update ExportResourceMappingConfig - Liver Diseases
</commit_message>
<xml_diff>
--- a/src/main/groovy/projects/gecco/crf/GroovyGeneratorFromTemplate/values_CardiovascularDiseases.xlsx
+++ b/src/main/groovy/projects/gecco/crf/GroovyGeneratorFromTemplate/values_CardiovascularDiseases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Macedo\PycharmProjects\ngu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0F36CC-F24E-4B84-AAB0-6410A2B5FCE3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9CD516-A823-4A46-8421-7B5BD3B07053}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1536,7 +1536,7 @@
   <dimension ref="A1:K73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Debug diseases and organ transplant
</commit_message>
<xml_diff>
--- a/src/main/groovy/projects/gecco/crf/GroovyGeneratorFromTemplate/values_CardiovascularDiseases.xlsx
+++ b/src/main/groovy/projects/gecco/crf/GroovyGeneratorFromTemplate/values_CardiovascularDiseases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Macedo\PycharmProjects\ngu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Macedo\IdeaProjects\kairos-fhir-dsl-mapping-example\src\main\groovy\projects\gecco\crf\GroovyGeneratorFromTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9CD516-A823-4A46-8421-7B5BD3B07053}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876A3564-916B-4B24-8219-8492F9AADDB3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Herzrhythmusstörungen</t>
   </si>
   <si>
-    <t>COV_GECCO_HERZKREISLAUF_HERZRHYTHMUSSTÖRUNGEN</t>
-  </si>
-  <si>
     <t>Leidet der/die Patient*in an Herzrhythmusstörungen?</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>KoronareHerzkrankheit</t>
+  </si>
+  <si>
+    <t>COV_GECCO_HERZKREISLAUF_HERZRHYTHMUSSTOERUNGEN</t>
   </si>
 </sst>
 </file>
@@ -1535,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1557,25 +1557,25 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="E1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
@@ -1586,13 +1586,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="11">
         <v>38341003</v>
@@ -1601,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -1610,16 +1610,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="11">
         <v>399211009</v>
@@ -1637,25 +1637,25 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="11">
         <v>698247007</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>7</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -1664,25 +1664,25 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="11">
         <v>84114007</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>10</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -1690,25 +1690,25 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="11">
         <v>399957001</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -1717,25 +1717,25 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="11">
         <v>399261000</v>
       </c>
       <c r="F7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -1744,25 +1744,25 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="11">
         <v>53741008</v>
       </c>
       <c r="F8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>19</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -1771,25 +1771,25 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="11">
         <v>64586002</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>

</xml_diff>